<commit_message>
Altered NUMER_OF_MONTHS input rules
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,22 +456,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>‘Once-in-a-lifetime caper’: How did the U.S. catch ‘El Mayo,’ the Sinaloa cartel’s top boss?</t>
+          <t>Editorial: LAUSD students’ scores are bouncing back — thanks to teachers</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Despite more than four decades on the run as one of the world’s most wanted fugitives, Mexican drug kingpin Ismael “El Mayo” Zambada had never spent a single night in jail -- until now.</t>
+          <t>The latest test scores for L.A. students are encouraging — but not yet time for a full-throated cheer because they are still below pre-pandemic levels.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2 hours ago</t>
+          <t>July 28, 2024</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>cb1adc6f-fce2-49ed-9b75-c42fac52005a</t>
+          <t>a594b684-67c7-4296-beb7-90175a6e0af1</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -484,22 +484,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Juixxe the viral TikToker takes on street vendor rights and dreams</t>
+          <t>Tim Vanderhook</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Juixxe surprises day laborers with cash and Disneyland trips, as seen by millions in viral videos. Now the TikToker is defending street vendor livelihoods.</t>
+          <t>Tim Vanderhook is a visionary entrepreneur and the driving force behind Viant Technology Inc (NASDAQ: DSP), a leading advertising technology company he co-founded with his brother Chris.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 28, 2024</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>488082b4-71b8-4819-8db9-e5eaf052dd11</t>
+          <t>8f35108c-afcf-423a-ad1e-c236304d491a</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -512,22 +512,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Most of Wall Street leaps in a widespread rally, from big stocks to small</t>
+          <t>Sasha Strauss</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Wall Street rallied after encouraging reports on inflation and on strong profits at 3M and other big U.S. companies.</t>
+          <t>Sasha Strauss is a distinguished brand strategy expert, educator and speaker renowned for his 25-year career shaping brands globally.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 28, 2024</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>c6814410-8a69-4a97-ac85-716e9a2b59d2</t>
+          <t>a0a3ce09-3328-4a8d-a484-ec40f182240a</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -540,26 +540,26 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>After 57 years of open seating, is Southwest changing its brand?</t>
+          <t>Sona Shah</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>The popular low-cost airline Southwest announced major changes this week, including a switch from open to assigned seating that could ruffle feathers among loyal travelers.</t>
+          <t>Sona Shah founded My Private Professor (MPP) to democratize access to academic resources, leveraging her expertise in business litigation and passion for education.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 28, 2024</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>6075d251-f38d-470c-88bf-57e9ca131144</t>
+          <t>f5e63fc1-6457-432f-bc2c-0ad9c2a19651</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -568,22 +568,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>From Let’s Go Brandon to Let’s Go Brenda. Trump merch sellers say they’ll be just fine after Biden exit</t>
+          <t>Lucy Santana</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>The Trump campaign embraced the anti-Biden slogan Let’s Go Brandon. Is it still effective after Biden dropped out?</t>
+          <t>Lucy Santana has led Girls Inc. of Orange County for over 20 years, transforming it into a leading chapter nationally.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 28, 2024</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>e5bc1f70-03de-48d6-9457-03e3b0bcbb2f</t>
+          <t>42b52a4b-ff6c-4f21-961f-6b53084af30d</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -596,22 +596,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Warner Bros. Discovery sues NBA over new media rights deal, saying it matched Amazon</t>
+          <t>Michael J. Beals</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>The parent company of the TNT cable network asserts the NBA breached its current deal by allegedly refusing to honor rights to match an offer from Amazon.</t>
+          <t>Dr. Michael J. Beals has served as president of Vanguard University (VU) for 10 years, guiding Orange County’s oldest four-year university to significant growth and achievement.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 28, 2024</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>a5f6303d-3bd5-4a7e-9c05-25594e669206</t>
+          <t>238e78cd-3ddb-4faf-adda-dc988d4b96ce</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -624,22 +624,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Prosecutors urge judge not to toss out Trump’s hush money conviction on immunity claim</t>
+          <t>Emil Davtyan</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Prosecutors urge judge to uphold Donald Trump’s hush money conviction, saying it should stand despite a Supreme Court ruling on presidential immunity.</t>
+          <t>Emil Davtyan, the founder and CEO of D.Law, deserves recognition for his exceptional leadership and dedication to advocating for California workers’ rights.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 28, 2024</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1418b912-bbc8-4ea0-a240-28b9d1f4d840</t>
+          <t>6ce63d7d-3b1c-41b7-95f1-486c79c28426</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -652,22 +652,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>FAA clears SpaceX’s Falcon 9 rocket for launch after malfunction</t>
+          <t>Prioritizing Tech Innovation &amp; Talent Retention</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>The Federal Aviation Administration on Friday cleared SpaceX’s workhorse Falcon 9 rocket to resume launch operations as it continues a probe into a failure of the rocket’s second stage this month.</t>
+          <t>Moderator: Brian Hegarty Principal, L.A.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 28, 2024</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4f0e351a-b6fe-4631-b8fa-c87c33a87ad2</t>
+          <t>e69e26db-b569-443d-ae18-201df0e5d4ef</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -680,12 +680,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>What we know so far about the attack on France’s rail network ahead of Olympics opening</t>
+          <t>Column: 99 years after the Scopes ‘monkey trial,’ religious fundamentalism still infects our schools</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>French transport was thrust into chaos before the Paris Olympics’ opening ceremony after coordinated ‘malicious acts’ upended high-speed train lines.</t>
+          <t>The Scopes trial made anti-evolutionists look ridiculous, but they haven’t gone away.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -695,7 +695,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>c784df26-aa07-4e21-80c3-dae290d304e1</t>
+          <t>3e03fc44-a137-4353-a803-e775a5b8d6a3</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -708,22 +708,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Newsom calls on Oakland to allow more police chases, stop suspects from ‘fleeing with impunity’</t>
+          <t>Homeless encampment cleanups do little to change numbers of people on the street, study finds</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>California Gov. Gavin Newsom criticized an Oakland policy that limits when police can engage in vehicle pursuits, warning of “extreme danger to the public in allowing criminals to act with impunity.”</t>
+          <t>Three new studies shed new light on homelessness in Los Angeles, painting a mostly grim picture, with some glimmers of hope.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 24, 2024</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>35e20959-17eb-4184-a8fc-2d25c669f870</t>
+          <t>42ce960d-b14c-4eb3-8e11-71996ab67252</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -736,22 +736,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>‘Deadpool &amp; Wolverine’ box office gives an R-rated boost to Marvel</t>
+          <t>LAUSD test scores rise in math and English, positive marks after pandemic setbacks</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>After a string of box office misses, Marvel is looking to ‘Deadpool &amp; Wolverine’ to bring an R-rated X-Men-powered refresh to the franchise.</t>
+          <t>Supt. Alberto Carvalho said the nation’s second-largest school system has seen across-the-board improvement in math and English scores in every grade.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 23, 2024</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>be7dc242-c230-40d4-be51-863d8bb8c7d7</t>
+          <t>ecf17e92-5466-441d-93c6-75004db30934</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -764,22 +764,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Well-known stock trader and his L.A. firm are charged with fraud and market manipulation</t>
+          <t>Boiling Point: Living in Death Valley</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Federal prosecutors and securities regulators in Los Angeles announced charges Friday against prominent short-seller Andrew Left, alleging he made millions of dollars of ill-gotten gains.</t>
+          <t>Death Valley residents talk about how they deal with extreme heat every day in the summer</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 23, 2024</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>8cd29868-0572-4e7b-ae62-3465ca9249d9</t>
+          <t>4b55a9fa-6af2-420a-b18c-0e7239eaf453</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -792,22 +792,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Olympics 2024: Celine Dion closes dazzling opening ceremony atop the Eiffel Tower</t>
+          <t>The 22 best spots to nerd out in L.A.</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Read analysis of the Paris Olympics opening ceremony from our television writers, who weighed in on the spectacle held on the Seine.</t>
+          <t>Whether you’re fiercely into tabletop games, robots, pinball, dinosaurs, space, comic books or close-up magic, here’s where you can find your people.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 23, 2024</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>293a5dd9-cab9-4b41-905d-4896ea442bb5</t>
+          <t>77c0375a-7cf1-4ce9-8cfb-7bd04e4cdbb5</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -820,22 +820,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Fed’s preferred inflation gauge cools, adding to likelihood of a September rate cut</t>
+          <t>Carvalho, who unplugged school AI chatbot, wants task force to tell him what went wrong</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>The Federal Reserve’s favored inflation measure remained low last month, bolstering evidence that price pressures are steadily cooling and setting the stage for the Fed to begin cutting interest rates this fall.</t>
+          <t>Independent experts will be asked to look at what went amiss with LAUSD’s AI effort and helped plan next steps in the ongoing but stalled strategy.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 23, 2024</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>8fa883c2-c67d-4f88-952c-41cbe9248097</t>
+          <t>1fe90465-e048-4778-a395-5d550b966ab4</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -848,22 +848,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Newsom’s order to clear encampments could backfire</t>
+          <t>Could AI robots with lasers make herbicides — and farm workers — obsolete?</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Critics worry that cities will lean into criminalizing and further marginalizing unhoused people, worsening the crisis.</t>
+          <t>A shift from harmful herbicides to intelligent robots would have far-reaching consequences for California’s $50-billion agriculture industry.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 22, 2024</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>c42019ed-2b3b-4c2f-b102-6a12c0af07a0</t>
+          <t>e06936f8-83c8-4160-a23c-f3db6ee37fc5</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -876,22 +876,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Editorial: California’s cannabis regulator is failing the legal marijuana market</t>
+          <t>Robert T. Braithwaite, Channing Hamlet and Daniel A. Platt Share Insights on the Healthcare, Biotech and Life Sciences Landscape in 2024</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Legal pot is tested and safer for consumers. But the Department of Cannabis Control’s failure to address lab fraud and tainted items undercuts the legal market.</t>
+          <t>The Healthcare, Biotech &amp; Life Sciences Roundtable panel is produced by the L.A.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 22, 2024</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>873d88d1-172b-4173-8d17-68319ee1e73e</t>
+          <t>d1f0fed9-a126-4f51-8882-3109149ccf5a</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -904,22 +904,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Column: 99 years after the Scopes ‘monkey trial,’ religious fundamentalism still infects our schools</t>
+          <t>Usha Vance: From San Francisco corporate lawyer to MAGA’s potential second lady</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>The Scopes trial made anti-evolutionists look ridiculous, but they haven’t gone away.</t>
+          <t>The California native and daughter of Indian academics has devoted her life to amassing the kind of elite professional credentials that draw scorn from GOP populists.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 19, 2024</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>81850c28-f3f2-4af6-8e66-3113796b12d6</t>
+          <t>7ca088c4-2128-4f44-b0bf-2473d99473ea</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -932,22 +932,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Opinion: Inglewood needs the people mover, Rep. Waters</t>
+          <t>These California counties endured the nation’s longest streaks of excessive heat</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>The plan to add a three-station connector to the Metro K line has been vetted, and its funding is all but secured. It puts Inglewood on the cusp of transit equity and environmental justice.</t>
+          <t>Several California communities near the Arizona border had the longest streak in the nation of days that hit 90 degrees or higher in 2022, according to new U.S. Census data.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 19, 2024</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0038b837-872e-437b-9e6a-d6a9755af24f</t>
+          <t>8cdc3a04-c97d-4940-9bed-c2bb0ba9705e</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -960,22 +960,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Don’t feed the meter. Save money and buy a parking permit at these L.A. and O.C. beaches</t>
+          <t>Review: ‘Tartuffe: Born Again’ in the American South kicks up its heels at Theatricum Botanicum</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>If you’re a frequent beachgoer, it would be cheaper to purchase a parking permit than to park on the street. Here are the cities in L.A. and Orange counties offering permits.</t>
+          <t>Freyda Thomas adapts Moliere’s ‘Tartuffe’ with an American twist in a winning production at Topanga’s beloved Will Geer Theatricum Botanicum.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 19, 2024</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>eda0c257-a3b4-4e8b-9040-7300c3b68b50</t>
+          <t>d313955b-74fc-49cd-952f-4984d19721ad</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -988,22 +988,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Benched by the NBA, Warner Bros. Discovery boss David Zaslav faces tough questions</t>
+          <t>UC regents ban views on Israel, other political opinion from university homepages</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>“They can’t go on like this,” Bank of America analyst Jessica Reif Ehrlich said, referring to the lagging stock and string of missteps by Warner Bros. Discovery boss David Zaslav.</t>
+          <t>UC regents voted Wednesday to ban views on political opinions from main campus homepages. Opinions may be posted on other pages but it must be made clear they aren’t official UC views.</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 18, 2024</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2c10c2a0-512f-4b64-bf4e-5a3ba688c9eb</t>
+          <t>e3543ab1-6a22-4a20-b75c-f397a8b47986</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1016,22 +1016,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>California home insurance program accused of selling policies with subpar fire coverage</t>
+          <t>For China, Trump rally shooting is more evidence of America’s demise</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Filed on behalf of more than 365,000 policy holders, the class-action lawsuit accuses the state’s insurance of last resort of unlawfully selling subpar fire insurance policies.</t>
+          <t>America’s biggest rival says Trump shooting symbolizes dwindling power and hypocrisy of American democracy and global leadership.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 17, 2024</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>312f7475-e2d9-43f1-9929-5d1bf9ea2899</t>
+          <t>f35fac03-33c7-4f85-8f51-884278b4402c</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1044,22 +1044,22 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Letters to the Editor: Dear Mr. President: Thank you for everything. You’ve earned your rest</t>
+          <t>Former Stanford dean, now local council member, apologizes for affair with student</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Americans are ‘forever grateful to you for your wisdom, integrity, grit, compassion and political savvy,’ a reader writes to President Biden.</t>
+          <t>Palo Alto City Council Member Julie Lythcott-Haims apologized for the romantic relationship she had with a Stanford undergrad more than a decade ago when she served as university dean.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 15, 2024</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>a787d610-f34e-47ef-8fac-ec2bd2fb9bbf</t>
+          <t>de7a1752-e71d-454f-a922-692414ca5b36</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1072,22 +1072,22 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Letters to the Editor: The CrowdStrike fiasco has shown us what we’ve lost as humans</t>
+          <t>Opinion: J.D. Vance’s book ‘Hillbilly Elegy’ was a con job. Don’t let it slide</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>If we continue to abdicate our human abilities to tech overlords, expect more problems like the CrowdStrike failure, warns a reader.</t>
+          <t>The running mate for Donald Trump showed in his 2016 memoir that he doesn’t understand or respect the working class. The media should call him out on that.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 15, 2024</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>4e026d31-4d89-4afb-a6c7-a72be46aeb44</t>
+          <t>1fc1abb6-6e0a-480b-ac78-9a1fb47f161c</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -1100,22 +1100,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Can the Paris Summer Olympics give Peacock the streaming boost it needs?</t>
+          <t>UC regents: Protests yes, encampments no. Campus rules must be consistently enforced</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Peacock will have 5,000 hours of live coverage which is aimed at bringing in more subscribers to the platform.</t>
+          <t>Rich Leib, outgoing chair of the UC Board of Regents, says encampments should be banned, but protests that follow campus rules are welcomed as free speech. Many regents, senior leaders agree.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 15, 2024</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>fdac62a4-6eef-4957-b1ce-180f9c1e636e</t>
+          <t>17bc38cc-cf69-4560-a1c1-b31329345e0d</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1128,22 +1128,22 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Column: If a driverless taxi pulls up to a senior center, will anyone brave a ride?</t>
+          <t>There’s no crying in baseball, but there are plenty of great baseball books</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Despite some trepidation -- and fear of mishaps -- these seniors rejected human drivers and climbed into driverless cars. What happened next may surprise you</t>
+          <t>A new biography of Clayton Kershaw, a history of Chavez Ravine, a reevaluation of a Negro League star and more book recommendations for baseball fans.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 13, 2024</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>30a475fa-af4c-4c99-b9d1-0df1beea0ed5</t>
+          <t>c61bf178-e69a-43c0-a1d6-6654cdf04d9e</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1156,22 +1156,22 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Is this the solution to California’s soaring insurance prices due to wildfire risk?</t>
+          <t>Pricey camps. Family favors. Early dashes from work. How do parents survive summer?</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>The insurance industry will soon have the ability to use wildfire models when setting rates. Homeowners in high risk areas already know how these models have made policies hard to get and hard to afford.</t>
+          <t>The scramble for summer child care is no easy feat for working parents. Families must weave together summer camps, friendly favors and leeway at work — often at high cost.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 12, 2024</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>503f6ee2-d970-4b76-afe0-cbb56a12ec5a</t>
+          <t>7bbe742a-17f9-448e-b699-1fe49461f450</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -1184,22 +1184,22 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Opinion: Elon Musk and Peter Thiel backed Trump and Vance. What would their ticket do for tech?</t>
+          <t>Cal Poly Humboldt president to step down months after campus crackdowns</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>If the GOP takes the White House, that likely means mixed results for regulation of Big Tech.</t>
+          <t>Cal Poly Humboldt University President Tom Jackson Jr. announced Thursday that he is stepping down after a five-year run that included national attention this spring over a campus crackdown on pro-Palestinian protests.</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 12, 2024</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>b21bc390-4b4e-4cb5-87a5-6f377240499d</t>
+          <t>93412ffc-c1a0-4a30-878d-44402d8941e1</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1212,22 +1212,22 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Mexican cartel leader known as “El Mayo” pleads not guilty in federal court</t>
+          <t>Editorial: L.A. County shows L.A. city that reform doesn’t have to be hard</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Ismael ‘El Mayo’ Zambada and Joaquín Guzmán López, two of Mexico’s most-wanted men, were arrested at an El Paso airport, two sources familiar with the situation told the Los Angeles Times.</t>
+          <t>While the L.A. City Council dithered over the details and delayed changes that could affect their power, county leaders forged ahead with a comprehensive governance reform ballot proposal.</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>July 25, 2024</t>
+          <t>July 11, 2024</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>83572fd6-cfff-4a60-b066-1bab5538c94c</t>
+          <t>2eb4fd54-e6de-4eca-894d-71445666306f</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1240,22 +1240,22 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Billy Ray Cyrus doubles down on anger at Firerose after audio of heated argument leaks</t>
+          <t>Supt. Carvalho moves ahead with troubled AI effort despite collapse of tech contractor</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Billy Ray Cyrus voices more animosity toward estranged wife Firerose after he could be heard cursing her out in leaked audio. ‘I was at my wit’s end,’ he writes.</t>
+          <t>LAUSD unplugged chatbot after collapse of company that created it, but Carvalho says other features remain to help students. Most schools don’t yet have it.</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>July 26, 2024</t>
+          <t>July 11, 2024</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>676a2bbd-bc51-41b3-b880-5f05d73cf9c2</t>
+          <t>a9850ec3-2d59-4127-9728-29d66ab52ae7</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1268,28 +1268,252 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Primior Agrees To Be Acquired By Grillit Inc.</t>
+          <t>Column: Investing through index funds is more popular than ever, so why is it becoming controversial?</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Real estate private equity investment firm Primior agreed to be acquired by Grillit Inc. in a transaction valued at $30 million on July 22.</t>
+          <t>More Americans own stocks than ever before, yet the passive index funds they favor are facing increasing partisan criticism. Here’s why</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>July 25, 2024</t>
+          <t>July 10, 2024</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2ce4b37f-4341-4eee-a4e9-5930873c1bd2</t>
+          <t>5bec0f87-6b06-496c-b27d-6d010db2c6cf</t>
         </is>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>USC President Carol Folt’s contract is renewed, but university won’t say for how long</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>USC President Carol Folt, who has drawn praise for expanding student programs and boosting athletics but criticism for her handling of pro-Palestinian protests, has received an extension to her five-year contract by university trustees.</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>July 09, 2024</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>b711a767-39e3-414b-9d3c-c4a12c7a35ee</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Column: A Trump judge blocks another pro-worker Biden initiative, this one involving noncompete clauses</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>The Federal Trade Commission banned non-compete clauses, which block workers from moving to better jobs. A Trump-appointed judge has blocked it--of course</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>July 09, 2024</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>d87bdd3a-b65f-4c5b-9810-96ad0b179301</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Meet the Californians serving in the first class of the American Climate Corps</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>The White House has sworn in more than 9,000 members of the American Climate Corps. In California, they’re managing wildfires, installing solar panels and more.</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>July 09, 2024</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>b9b63e4a-ab90-42d6-b46c-9a29e4092645</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Alberto Carvalho: Bold post-COVID-lockdown school leader</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Alberto Carvalho brings a big resume and big style to the Los Angeles Unified School District. High hopes ride on him as students emerge from the COVID-19 pandemic.</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>July 07, 2024</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>114eb2a7-9545-4bec-abb0-7875160bc445</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Your guide to Proposition 2: Education bond</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>School bond supports say the money is direly needed to help fund repairs and upgrades at thousands of California public elementary, middle and high schools and community colleges.</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>July 05, 2024</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>39fa7719-691c-45ef-85b1-39dee11e7311</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Biden vows to keep running as signs point to rapidly eroding support on Capitol Hill</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>President Biden vows to keep running for reelection, rejecting pressure from within his Democratic Party to withdraw after his poor debate performance.</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>July 03, 2024</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>28d786bc-56c1-4df2-ae7b-dd56617ae09b</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>LAUSD shelves its hyped AI chatbot to help students after collapse of firm that made it</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>LAUSD sidelines “Ed,” an AI chatbot, after a splashy kick-off featuring a company that has now tanked. District also is dealing with another data breach.</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>July 03, 2024</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>e1375478-7b25-4bb3-9e21-39b3c0939df9</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Opinion: Fentanyl could fuel another cycle of loss in L.A.’s Black communities. It doesn’t have to</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Opioid overdoses are depriving hundreds of thousands of children of parents, with especially dire consequences for Black families in Southern California.</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>July 02, 2024</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>dbdb6af0-cf99-44be-973b-73b9e63494c5</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>